<commit_message>
Added m-ft conversion to Tables.xlsx
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
   <si>
     <t>A</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>Limit</t>
+  </si>
+  <si>
+    <t>1m = 3.281ft</t>
   </si>
 </sst>
 </file>
@@ -610,7 +613,7 @@
   <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,6 +1177,11 @@
       </c>
       <c r="G17">
         <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Group calculation, table_depth_index, unittests.
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -6125,8 +6125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="Z23" sqref="Z23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>